<commit_message>
view book by category
</commit_message>
<xml_diff>
--- a/Myshop/data/BookStoreData.xlsx
+++ b/Myshop/data/BookStoreData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\scr\Windows\Project-Myshop\Myshop\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\Project-Myshop\Myshop\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BA415EA-4B2D-41C8-874E-5A1D98C0D2E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A02CEE07-27B7-4CA4-B292-3BB4BF6C7CE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="3276" windowWidth="17280" windowHeight="9420" activeTab="1" xr2:uid="{AE188B15-61A8-499F-B711-103A85F37A54}"/>
+    <workbookView xWindow="5604" yWindow="696" windowWidth="17280" windowHeight="9420" activeTab="1" xr2:uid="{AE188B15-61A8-499F-B711-103A85F37A54}"/>
   </bookViews>
   <sheets>
     <sheet name="Category" sheetId="1" r:id="rId1"/>
@@ -28,8 +28,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -37,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="115">
   <si>
     <t>Name</t>
   </si>
@@ -298,6 +296,90 @@
   </si>
   <si>
     <t>BookImages/giolanhdaumua.jpg</t>
+  </si>
+  <si>
+    <t>Bìa cứng</t>
+  </si>
+  <si>
+    <t>Bìa mềm</t>
+  </si>
+  <si>
+    <t>Văn học</t>
+  </si>
+  <si>
+    <t>Lịch sử</t>
+  </si>
+  <si>
+    <t>Địa lý</t>
+  </si>
+  <si>
+    <t>categories</t>
+  </si>
+  <si>
+    <t>1, 9</t>
+  </si>
+  <si>
+    <t>2,11</t>
+  </si>
+  <si>
+    <t>2,10</t>
+  </si>
+  <si>
+    <t>2,3</t>
+  </si>
+  <si>
+    <t>2,6</t>
+  </si>
+  <si>
+    <t>1,3,10</t>
+  </si>
+  <si>
+    <t>2,3,12</t>
+  </si>
+  <si>
+    <t>2,7,9</t>
+  </si>
+  <si>
+    <t>1, 6,9</t>
+  </si>
+  <si>
+    <t>2, 10, 14</t>
+  </si>
+  <si>
+    <t>2, 10, 11</t>
+  </si>
+  <si>
+    <t>2,5</t>
+  </si>
+  <si>
+    <t>2,6,7</t>
+  </si>
+  <si>
+    <t>1,9,14</t>
+  </si>
+  <si>
+    <t>1,3</t>
+  </si>
+  <si>
+    <t>2,15,3</t>
+  </si>
+  <si>
+    <t>1,12</t>
+  </si>
+  <si>
+    <t>2,3,10</t>
+  </si>
+  <si>
+    <t>2,8,4</t>
+  </si>
+  <si>
+    <t>2,10,14,4</t>
+  </si>
+  <si>
+    <t>2,10,13</t>
+  </si>
+  <si>
+    <t>Nhiều tác giả</t>
   </si>
 </sst>
 </file>
@@ -657,10 +739,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{290BE860-30F5-441A-8C4E-FB148E24F7CF}">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:A16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -675,51 +757,76 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
         <v>10</v>
       </c>
     </row>
@@ -730,10 +837,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A3736BF-CD8D-4BC0-8556-439C55123192}">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -744,7 +851,7 @@
     <col min="4" max="4" width="26.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -763,8 +870,11 @@
       <c r="F1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -783,8 +893,11 @@
       <c r="F2">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -803,8 +916,11 @@
       <c r="F3">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -823,8 +939,11 @@
       <c r="F4">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -843,8 +962,11 @@
       <c r="F5">
         <v>30</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="41.4">
+      <c r="G5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="41.4">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -863,8 +985,11 @@
       <c r="F6">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="G6" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -883,8 +1008,11 @@
       <c r="F7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="G7" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -903,8 +1031,11 @@
       <c r="F8">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="G8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -923,8 +1054,11 @@
       <c r="F9">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="G9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -943,8 +1077,11 @@
       <c r="F10">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="G10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -963,8 +1100,11 @@
       <c r="F11">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="G11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -983,8 +1123,11 @@
       <c r="F12">
         <v>40</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="G12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>46</v>
       </c>
@@ -1003,8 +1146,11 @@
       <c r="F13">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="G13" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>48</v>
       </c>
@@ -1023,8 +1169,11 @@
       <c r="F14">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="G14" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>51</v>
       </c>
@@ -1043,8 +1192,11 @@
       <c r="F15">
         <v>7</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="G15" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>54</v>
       </c>
@@ -1063,8 +1215,11 @@
       <c r="F16">
         <v>8</v>
       </c>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="G16" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>57</v>
       </c>
@@ -1083,8 +1238,11 @@
       <c r="F17">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="G17" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>60</v>
       </c>
@@ -1103,8 +1261,11 @@
       <c r="F18">
         <v>10</v>
       </c>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="G18" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>62</v>
       </c>
@@ -1123,8 +1284,11 @@
       <c r="F19">
         <v>16</v>
       </c>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="G19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
         <v>68</v>
       </c>
@@ -1143,8 +1307,11 @@
       <c r="F20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="G20" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>71</v>
       </c>
@@ -1163,8 +1330,11 @@
       <c r="F21">
         <v>8</v>
       </c>
-    </row>
-    <row r="22" spans="1:6">
+      <c r="G21" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>74</v>
       </c>
@@ -1183,8 +1353,11 @@
       <c r="F22">
         <v>14</v>
       </c>
-    </row>
-    <row r="23" spans="1:6">
+      <c r="G22" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
         <v>77</v>
       </c>
@@ -1203,14 +1376,20 @@
       <c r="F23">
         <v>11</v>
       </c>
-    </row>
-    <row r="24" spans="1:6">
+      <c r="G23" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24" t="s">
         <v>80</v>
       </c>
       <c r="B24">
         <v>2005</v>
       </c>
+      <c r="C24" t="s">
+        <v>114</v>
+      </c>
       <c r="D24" t="s">
         <v>81</v>
       </c>
@@ -1220,8 +1399,11 @@
       <c r="F24">
         <v>40</v>
       </c>
-    </row>
-    <row r="25" spans="1:6">
+      <c r="G24" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25" t="s">
         <v>82</v>
       </c>
@@ -1239,6 +1421,9 @@
       </c>
       <c r="F25">
         <v>6</v>
+      </c>
+      <c r="G25" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>